<commit_message>
Sync full website assets
</commit_message>
<xml_diff>
--- a/LR_tagged_download.xlsx
+++ b/LR_tagged_download.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coo/Desktop/LR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7EF2B0-D0BE-E44E-BBCF-4AB5ACE536A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FEAAE8-1DDF-8E44-A032-57A839F0692C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1439,7 +1439,7 @@
   <dimension ref="A1:M92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>